<commit_message>
Added ranges to the code, tempor.
</commit_message>
<xml_diff>
--- a/protocols/Group_Ass.xlsx
+++ b/protocols/Group_Ass.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
   <si>
     <t>Members</t>
   </si>
@@ -289,7 +289,10 @@
     <t>Object Detection subsystem, First Library</t>
   </si>
   <si>
-    <t>TO-DO</t>
+    <t>LightSensor Beacon</t>
+  </si>
+  <si>
+    <t>LightSensor code</t>
   </si>
 </sst>
 </file>
@@ -626,7 +629,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -741,16 +744,13 @@
     <xf numFmtId="49" fontId="4" fillId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="59" fontId="4" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -934,7 +934,7 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>23.000000</c:v>
+                  <c:v>24.000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6.000000</c:v>
@@ -1304,13 +1304,13 @@
               <c:numCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>26.000000</c:v>
+                  <c:v>28.000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.000000</c:v>
+                  <c:v>1.000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.000000</c:v>
+                  <c:v>0.000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="D4" s="8">
         <f>COUNTIF(K19:K47,"*LB*")</f>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" ht="23" customHeight="1">
@@ -2748,7 +2748,7 @@
       </c>
       <c r="F12" s="16">
         <f>COUNTIF(J19:J47,"=DONE")</f>
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" ht="22.5" customHeight="1">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="F13" s="18">
         <f>COUNTIF(J19:J47,"=WIP")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" ht="22.5" customHeight="1">
@@ -2766,7 +2766,7 @@
       </c>
       <c r="F14" s="19">
         <f>COUNTIF(J19:J47,"=TO-DO")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" ht="22.6" customHeight="1">
@@ -3190,14 +3190,12 @@
       <c r="I41" s="28"/>
       <c r="J41" t="s" s="27">
         <f>IF(L41="WIP","WIP",IF(K41=L41,"TO-DO","DONE"))</f>
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K41" t="s" s="27">
         <v>82</v>
       </c>
-      <c r="L41" t="s" s="35">
-        <v>26</v>
-      </c>
+      <c r="L41" s="29"/>
     </row>
     <row r="42" ht="22.5" customHeight="1">
       <c r="G42" t="s" s="26">
@@ -3287,15 +3285,21 @@
       <c r="L46" s="34"/>
     </row>
     <row r="47" ht="22.6" customHeight="1">
-      <c r="G47" s="38"/>
-      <c r="H47" s="39"/>
+      <c r="G47" t="s" s="38">
+        <v>92</v>
+      </c>
+      <c r="H47" t="s" s="39">
+        <v>93</v>
+      </c>
       <c r="I47" s="40"/>
-      <c r="J47" t="s" s="41">
+      <c r="J47" t="s" s="39">
         <f>IF(L47="WIP","WIP",IF(K47=L47,"TO-DO","DONE"))</f>
-        <v>92</v>
-      </c>
-      <c r="K47" s="39"/>
-      <c r="L47" s="42"/>
+        <v>29</v>
+      </c>
+      <c r="K47" t="s" s="39">
+        <v>5</v>
+      </c>
+      <c r="L47" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>